<commit_message>
Testando códigos da web
</commit_message>
<xml_diff>
--- a/GoogleSheets/TesteParaC#V1.xlsx
+++ b/GoogleSheets/TesteParaC#V1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>testando</t>
   </si>
@@ -51,6 +51,24 @@
   </si>
   <si>
     <t>03/09/2025 22:53:42</t>
+  </si>
+  <si>
+    <t>paulo mandou abaixar o volume</t>
+  </si>
+  <si>
+    <t>06/09/2025 23:47:00</t>
+  </si>
+  <si>
+    <t>testandooo</t>
+  </si>
+  <si>
+    <t>06/09/2025 23:47:43</t>
+  </si>
+  <si>
+    <t>testeee oii</t>
+  </si>
+  <si>
+    <t>06/09/2025 23:47:59</t>
   </si>
 </sst>
 </file>
@@ -96,7 +114,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -165,6 +183,30 @@
         <v>12</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Adicionando dados por um array
</commit_message>
<xml_diff>
--- a/GoogleSheets/TesteParaC#V1.xlsx
+++ b/GoogleSheets/TesteParaC#V1.xlsx
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" fullPrecision="1"/>
   <extLst>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
@@ -25,13 +25,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>testando</t>
+  </si>
+  <si>
+    <t>07/09/2025 17:16:35</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
@@ -56,8 +69,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,14 +386,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <headerFooter/>
 </worksheet>
+</file>
+
+<file path=EPPlusLicense.txt>This workbook was created with the EPPlus library, licensed to DanielGalleazzo under the Polyform Noncommercial license, see https://polyformproject.org/licenses/noncommercial/1.0.0
+For more information about EPPlus, see https://epplussoftware.com/
+
 </file>
</xml_diff>